<commit_message>
- updated specifications and drawings - updated readme
</commit_message>
<xml_diff>
--- a/doc/Revision_Specifications.xlsx
+++ b/doc/Revision_Specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_boot\Seltron\revision\revision\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D8D264-2428-484A-91C6-84104A317E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880565FB-42DC-4A07-8228-B8C38D73A5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Document status:</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>Signature</t>
+  </si>
+  <si>
+    <t>Reserved</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,18 +569,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -950,11 +977,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -976,53 +1051,14 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1033,25 +1069,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1070,9 +1094,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1092,22 +1209,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>720436</xdr:colOff>
+      <xdr:colOff>459442</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>138545</xdr:rowOff>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>193435</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>3385</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>133119</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Slika 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB312AC1-48C1-9268-6EA1-E4529F3E4077}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C5D058-20A3-C6B1-632A-B76AA74FEE02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,8 +1240,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16154400" y="332509"/>
-          <a:ext cx="8630854" cy="6001588"/>
+          <a:off x="9962030" y="257735"/>
+          <a:ext cx="10532177" cy="6992471"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1405,30 +1522,30 @@
       <selection activeCell="E5" sqref="E5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.44140625" customWidth="1"/>
-    <col min="2" max="11" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" customWidth="1"/>
+    <col min="2" max="11" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="36" t="s">
+    <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-    </row>
-    <row r="3" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1438,16 +1555,16 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
-    </row>
-    <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1457,133 +1574,127 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="31"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="28"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E8" s="28"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="31"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E9" s="28"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="31"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E10" s="28"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E11" s="28"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="31"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E12" s="28"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E13" s="28"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="31"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E14" s="28"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -1592,6 +1703,12 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1600,291 +1717,336 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB689FC-E53B-4F42-BD0A-17CBB93FB776}">
-  <dimension ref="C1:G31"/>
+  <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="2.21875" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="69.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="1" max="2" width="2.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="10" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="3:7" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="21" t="s">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="47.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="3:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C3" s="22" t="s">
+    <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="36"/>
+      <c r="C3" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="49">
         <v>0</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="49">
         <v>1</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="50" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C4" s="23" t="s">
+    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="36"/>
+      <c r="C4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="53">
         <v>1</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="53">
         <v>1</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="54" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="23" t="s">
+    <row r="5" spans="2:7" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="36"/>
+      <c r="C5" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="53">
         <v>2</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="53">
         <v>1</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="C6" s="23" t="s">
+    <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="59"/>
+      <c r="C6" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34">
+        <v>3</v>
+      </c>
+      <c r="F6" s="34">
+        <v>5</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="37"/>
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D7" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E7" s="57">
         <v>8</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F7" s="57">
         <v>4</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G7" s="58" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C7" s="23" t="s">
+    <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="37"/>
+      <c r="C8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E8" s="40">
         <v>12</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F8" s="40">
         <v>4</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G8" s="41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="23" t="s">
+    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="37"/>
+      <c r="C9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D9" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E9" s="40">
         <v>16</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F9" s="40">
         <v>4</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G9" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="23" t="s">
+    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D10" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E10" s="40">
         <v>20</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F10" s="40">
         <v>4</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G10" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C10" s="23" t="s">
+    <row r="11" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="37"/>
+      <c r="C11" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D11" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E11" s="40">
         <v>24</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F11" s="40">
         <v>4</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G11" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="23" t="s">
+    <row r="12" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="37"/>
+      <c r="C12" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D12" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E12" s="40">
         <v>28</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F12" s="40">
         <v>1</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G12" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="23" t="s">
+    <row r="13" spans="2:7" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="37"/>
+      <c r="C13" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D13" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E13" s="40">
         <v>29</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F13" s="40">
         <v>1</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G13" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C13" s="24" t="s">
+    <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="37"/>
+      <c r="C14" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D14" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E14" s="40">
         <v>30</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F14" s="40">
         <v>64</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G14" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C14" s="24" t="s">
+    <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="37"/>
+      <c r="C15" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D15" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E15" s="40">
         <v>94</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F15" s="40">
         <v>32</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G15" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="3:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="25" t="s">
+    <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="37"/>
+      <c r="C16" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D16" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E16" s="45">
         <v>126</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F16" s="45">
         <v>8</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G16" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="37"/>
+      <c r="C17" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34">
+        <v>134</v>
+      </c>
+      <c r="F17" s="34">
+        <v>122</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- updated revision specs
</commit_message>
<xml_diff>
--- a/doc/Revision_Specifications.xlsx
+++ b/doc/Revision_Specifications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_boot\Seltron\revision\revision\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_app\Seltron\revision\revision\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880565FB-42DC-4A07-8228-B8C38D73A5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAA668B-26AD-4FC5-9369-E35D66A842F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,10 +175,6 @@
     <t>Image CRC</t>
   </si>
   <si>
-    <t>Image CRC
-Image CRC is calculated pass header</t>
-  </si>
-  <si>
     <t>Hash</t>
   </si>
   <si>
@@ -428,6 +424,24 @@
   </si>
   <si>
     <t>Reserved</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Image CRC
+Image CRC is calculated pass header
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE: In case encryption is enabled, then image CRC is calculated on encrypted image! For more info, look at the app_sign_tool!</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1068,14 +1082,107 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1093,99 +1200,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1216,8 +1230,8 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>133119</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1530,19 +1544,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1555,146 +1569,152 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="25"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
+      <c r="E5" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="47"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="47"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="47"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -1703,12 +1723,6 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1720,7 +1734,7 @@
   <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,278 +1757,278 @@
         <v>4</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="20"/>
+      <c r="C3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
+        <v>1</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="20"/>
+      <c r="C4" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="37">
+        <v>1</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20"/>
+      <c r="C5" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="37">
+        <v>2</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="43"/>
+      <c r="C6" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18">
+        <v>3</v>
+      </c>
+      <c r="F6" s="18">
+        <v>5</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="21"/>
+      <c r="C7" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="41">
+        <v>8</v>
+      </c>
+      <c r="F7" s="41">
+        <v>4</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="24">
+        <v>12</v>
+      </c>
+      <c r="F8" s="24">
+        <v>4</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="24">
+        <v>16</v>
+      </c>
+      <c r="F9" s="24">
+        <v>4</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="24">
+        <v>20</v>
+      </c>
+      <c r="F10" s="24">
+        <v>4</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="24">
+        <v>24</v>
+      </c>
+      <c r="F11" s="24">
+        <v>4</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="24">
+        <v>28</v>
+      </c>
+      <c r="F12" s="24">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="24">
+        <v>29</v>
+      </c>
+      <c r="F13" s="24">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="21"/>
+      <c r="C14" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="24">
+        <v>30</v>
+      </c>
+      <c r="F14" s="24">
+        <v>64</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="21"/>
+      <c r="C15" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="24">
+        <v>94</v>
+      </c>
+      <c r="F15" s="24">
+        <v>32</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="21"/>
+      <c r="C16" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="49">
-        <v>0</v>
-      </c>
-      <c r="F3" s="49">
-        <v>1</v>
-      </c>
-      <c r="G3" s="50" t="s">
+      <c r="D16" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="29">
+        <v>126</v>
+      </c>
+      <c r="F16" s="29">
+        <v>8</v>
+      </c>
+      <c r="G16" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="53">
-        <v>1</v>
-      </c>
-      <c r="F4" s="53">
-        <v>1</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="53">
-        <v>2</v>
-      </c>
-      <c r="F5" s="53">
-        <v>1</v>
-      </c>
-      <c r="G5" s="54" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="59"/>
-      <c r="C6" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34">
-        <v>3</v>
-      </c>
-      <c r="F6" s="34">
-        <v>5</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="57">
-        <v>8</v>
-      </c>
-      <c r="F7" s="57">
-        <v>4</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="37"/>
-      <c r="C8" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="40">
-        <v>12</v>
-      </c>
-      <c r="F8" s="40">
-        <v>4</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="37"/>
-      <c r="C9" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="40">
-        <v>16</v>
-      </c>
-      <c r="F9" s="40">
-        <v>4</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="40">
-        <v>20</v>
-      </c>
-      <c r="F10" s="40">
-        <v>4</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
-      <c r="C11" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="40">
-        <v>24</v>
-      </c>
-      <c r="F11" s="40">
-        <v>4</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
-      <c r="C12" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="40">
-        <v>28</v>
-      </c>
-      <c r="F12" s="40">
-        <v>1</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="40">
-        <v>29</v>
-      </c>
-      <c r="F13" s="40">
-        <v>1</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
-      <c r="C14" s="42" t="s">
+    <row r="17" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="21"/>
+      <c r="C17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="40">
-        <v>30</v>
-      </c>
-      <c r="F14" s="40">
-        <v>64</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="40">
-        <v>94</v>
-      </c>
-      <c r="F15" s="40">
-        <v>32</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="45">
-        <v>126</v>
-      </c>
-      <c r="F16" s="45">
-        <v>8</v>
-      </c>
-      <c r="G16" s="46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="37"/>
-      <c r="C17" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34">
+      <c r="D17" s="17"/>
+      <c r="E17" s="18">
         <v>134</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="18">
         <v>122</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2050,6 +2064,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- redefining image size
</commit_message>
<xml_diff>
--- a/doc/Revision_Specifications.xlsx
+++ b/doc/Revision_Specifications.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_app\Seltron\revision\revision\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_boot\Seltron\revision\revision\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAA668B-26AD-4FC5-9369-E35D66A842F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2B1B86-D5F6-4DF1-B9F9-70DFE95B4780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,9 +159,6 @@
 Version is coded same as SW version</t>
   </si>
   <si>
-    <t>Image size in bytes</t>
-  </si>
-  <si>
     <t>Image absolute address in case of "Custom" image type option.</t>
   </si>
   <si>
@@ -441,6 +438,23 @@
         <scheme val="minor"/>
       </rPr>
       <t>NOTE: In case encryption is enabled, then image CRC is calculated on encrypted image! For more info, look at the app_sign_tool!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Image size in bytes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE: This is only image size, without counting in size of header!</t>
     </r>
   </si>
 </sst>
@@ -1164,25 +1178,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1200,6 +1202,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1223,43 +1237,121 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>459442</xdr:colOff>
+      <xdr:colOff>299357</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
+      <xdr:rowOff>517072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>133119</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>59657</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Slika 2">
+        <xdr:cNvPr id="4" name="Slika 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C5D058-20A3-C6B1-632A-B76AA74FEE02}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B008DEF3-93ED-CA20-F9A2-7AF18AE1E678}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9962030" y="257735"/>
-          <a:ext cx="10532177" cy="6992471"/>
+          <a:off x="9797143" y="721179"/>
+          <a:ext cx="11312764" cy="7483928"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>585107</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>97349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Slika 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F80981E-9A8B-783A-389E-8AE9FF35D9C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10314214" y="8395606"/>
+          <a:ext cx="8259536" cy="6111707"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1544,19 +1636,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1569,39 +1661,39 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="58"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="60"/>
+      <c r="E5" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="45"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="46"/>
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
@@ -1612,7 +1704,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="51"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="46"/>
       <c r="G7" s="46"/>
       <c r="H7" s="46"/>
@@ -1623,7 +1715,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="45"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="46"/>
       <c r="G8" s="46"/>
       <c r="H8" s="46"/>
@@ -1634,7 +1726,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="45"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
@@ -1645,7 +1737,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="45"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="46"/>
       <c r="G10" s="46"/>
       <c r="H10" s="46"/>
@@ -1656,7 +1748,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="45"/>
+      <c r="E11" s="57"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
       <c r="H11" s="46"/>
@@ -1667,7 +1759,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="45"/>
+      <c r="E12" s="57"/>
       <c r="F12" s="46"/>
       <c r="G12" s="46"/>
       <c r="H12" s="46"/>
@@ -1678,7 +1770,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="45"/>
+      <c r="E13" s="57"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
       <c r="H13" s="46"/>
@@ -1689,7 +1781,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="45"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="46"/>
       <c r="G14" s="46"/>
       <c r="H14" s="46"/>
@@ -1700,21 +1792,15 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -1723,6 +1809,12 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1733,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB689FC-E53B-4F42-BD0A-17CBB93FB776}">
   <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,13 +1849,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1772,7 +1864,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="33">
         <v>0</v>
@@ -1790,7 +1882,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="37">
         <v>1</v>
@@ -1808,7 +1900,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="37">
         <v>2</v>
@@ -1823,7 +1915,7 @@
     <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="43"/>
       <c r="C6" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18">
@@ -1842,7 +1934,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="41">
         <v>8</v>
@@ -1872,13 +1964,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E9" s="24">
         <v>16</v>
@@ -1896,7 +1988,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="24">
         <v>20</v>
@@ -1911,10 +2003,10 @@
     <row r="11" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="24">
         <v>24</v>
@@ -1932,7 +2024,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="24">
         <v>28</v>
@@ -1950,7 +2042,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="24">
         <v>29</v>
@@ -1965,10 +2057,10 @@
     <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="24">
         <v>30</v>
@@ -1983,10 +2075,10 @@
     <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>25</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>26</v>
       </c>
       <c r="E15" s="24">
         <v>94</v>
@@ -2001,10 +2093,10 @@
     <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="28" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>32</v>
       </c>
       <c r="E16" s="29">
         <v>126</v>
@@ -2019,7 +2111,7 @@
     <row r="17" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="21"/>
       <c r="C17" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="18">

</xml_diff>

<commit_message>
- added encrypted image CRC field
</commit_message>
<xml_diff>
--- a/doc/Revision_Specifications.xlsx
+++ b/doc/Revision_Specifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_boot\Seltron\revision\revision\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2B1B86-D5F6-4DF1-B9F9-70DFE95B4780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BF7AAD-EABE-4393-90C4-5164CAEF27FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Document status:</t>
   </si>
@@ -424,8 +424,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Image CRC
-Image CRC is calculated pass header
+      <t xml:space="preserve">Image size in bytes
 </t>
     </r>
     <r>
@@ -437,12 +436,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>NOTE: In case encryption is enabled, then image CRC is calculated on encrypted image! For more info, look at the app_sign_tool!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Image size in bytes
+      <t>NOTE: This is only image size, without counting in size of header!</t>
+    </r>
+  </si>
+  <si>
+    <t>Encrypted image CRC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Image CRC
 </t>
     </r>
     <r>
@@ -454,7 +456,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>NOTE: This is only image size, without counting in size of header!</t>
+      <t>NOTE: Image CRC is calculated only on image part, wihtout header!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Encrypted image CRC
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE: Encrypted image CRC is calculated only on image part, without header. Applicable only for encrypted images, enc_type is not "none"!</t>
     </r>
   </si>
 </sst>
@@ -1178,13 +1197,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1202,18 +1233,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,23 +1255,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>299357</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>517072</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>59657</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>585107</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>97349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Slika 3">
+        <xdr:cNvPr id="5" name="Slika 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B008DEF3-93ED-CA20-F9A2-7AF18AE1E678}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F80981E-9A8B-783A-389E-8AE9FF35D9C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1261,7 +1280,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1275,8 +1294,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9797143" y="721179"/>
-          <a:ext cx="11312764" cy="7483928"/>
+          <a:off x="10314214" y="8395606"/>
+          <a:ext cx="8259536" cy="6111707"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1297,23 +1316,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>81642</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>585107</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>97349</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>172657</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>775608</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Slika 4">
+        <xdr:cNvPr id="2" name="Slika 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F80981E-9A8B-783A-389E-8AE9FF35D9C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5048A12-C717-ABA1-9B3B-7A8F74BC3B5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1322,7 +1341,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1336,8 +1355,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10314214" y="8395606"/>
-          <a:ext cx="8259536" cy="6111707"/>
+          <a:off x="9565822" y="149679"/>
+          <a:ext cx="12269406" cy="8096250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1636,19 +1655,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1661,14 +1680,14 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1680,20 +1699,20 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="56"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="46"/>
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
@@ -1704,7 +1723,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="45"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="46"/>
       <c r="G7" s="46"/>
       <c r="H7" s="46"/>
@@ -1715,7 +1734,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="57"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="46"/>
       <c r="G8" s="46"/>
       <c r="H8" s="46"/>
@@ -1726,7 +1745,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="57"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
@@ -1737,7 +1756,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="57"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="46"/>
       <c r="G10" s="46"/>
       <c r="H10" s="46"/>
@@ -1748,7 +1767,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="57"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
       <c r="H11" s="46"/>
@@ -1759,7 +1778,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="57"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="46"/>
       <c r="G12" s="46"/>
       <c r="H12" s="46"/>
@@ -1770,7 +1789,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="57"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
       <c r="H13" s="46"/>
@@ -1781,7 +1800,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="57"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="46"/>
       <c r="G14" s="46"/>
       <c r="H14" s="46"/>
@@ -1792,15 +1811,21 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -1809,12 +1834,6 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1823,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB689FC-E53B-4F42-BD0A-17CBB93FB776}">
-  <dimension ref="B1:G33"/>
+  <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1989,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="24">
         <v>16</v>
@@ -2000,13 +2019,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="24">
         <v>24</v>
@@ -2108,24 +2127,39 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="29">
+        <v>134</v>
+      </c>
+      <c r="F17" s="29">
+        <v>4</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="21"/>
+      <c r="C18" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18">
-        <v>134</v>
-      </c>
-      <c r="F17" s="18">
-        <v>122</v>
-      </c>
-      <c r="G17" s="19" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="18">
+        <v>138</v>
+      </c>
+      <c r="F18" s="18">
+        <v>118</v>
+      </c>
+      <c r="G18" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" s="9"/>
@@ -2153,6 +2187,9 @@
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- updated revision submodule
</commit_message>
<xml_diff>
--- a/doc/Revision_Specifications.xlsx
+++ b/doc/Revision_Specifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_boot\Seltron\revision\revision\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BF7AAD-EABE-4393-90C4-5164CAEF27FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D99E56C-C617-40A0-B85C-68514C79905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,21 @@
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
     <sheet name="Image header" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1197,25 +1208,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1233,6 +1232,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1655,19 +1666,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1680,14 +1691,14 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="58"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1699,20 +1710,20 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="60"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="45"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="46"/>
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
@@ -1723,7 +1734,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="51"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="46"/>
       <c r="G7" s="46"/>
       <c r="H7" s="46"/>
@@ -1734,7 +1745,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="45"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="46"/>
       <c r="G8" s="46"/>
       <c r="H8" s="46"/>
@@ -1745,7 +1756,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="45"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
@@ -1756,7 +1767,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="45"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="46"/>
       <c r="G10" s="46"/>
       <c r="H10" s="46"/>
@@ -1767,7 +1778,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="45"/>
+      <c r="E11" s="57"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
       <c r="H11" s="46"/>
@@ -1778,7 +1789,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="45"/>
+      <c r="E12" s="57"/>
       <c r="F12" s="46"/>
       <c r="G12" s="46"/>
       <c r="H12" s="46"/>
@@ -1789,7 +1800,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="45"/>
+      <c r="E13" s="57"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
       <c r="H13" s="46"/>
@@ -1800,7 +1811,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="45"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="46"/>
       <c r="G14" s="46"/>
       <c r="H14" s="46"/>
@@ -1811,21 +1822,15 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -1834,6 +1839,12 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1845,7 +1856,7 @@
   <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,7 +2166,7 @@
         <v>138</v>
       </c>
       <c r="F18" s="18">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G18" s="19" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
- updated definition of header image
</commit_message>
<xml_diff>
--- a/doc/Revision_Specifications.xlsx
+++ b/doc/Revision_Specifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SELTRON_AHD20W__2023\SOFTWARE\MASTER_SOURCE\STM32\ahd20w_sw_stm32l476_boot\Seltron\revision\revision\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D99E56C-C617-40A0-B85C-68514C79905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F51DEE-284C-4E2E-9731-10504B13A980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,9 +170,6 @@
 Version is coded same as SW version</t>
   </si>
   <si>
-    <t>Image absolute address in case of "Custom" image type option.</t>
-  </si>
-  <si>
     <t>Image header CRC value
 All fields beside CRC itself is part of the calculation.</t>
   </si>
@@ -486,6 +483,9 @@
       </rPr>
       <t>NOTE: Encrypted image CRC is calculated only on image part, without header. Applicable only for encrypted images, enc_type is not "none"!</t>
     </r>
+  </si>
+  <si>
+    <t>Image start address in flash</t>
   </si>
 </sst>
 </file>
@@ -1208,13 +1208,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1232,18 +1244,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1266,23 +1266,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>81642</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>122464</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>585107</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>97349</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>163287</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>649775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Slika 4">
+        <xdr:cNvPr id="4" name="Slika 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F80981E-9A8B-783A-389E-8AE9FF35D9C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE79C6F2-663A-5226-5AF9-B25DD13B85AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1291,7 +1291,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1305,8 +1305,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10314214" y="8395606"/>
-          <a:ext cx="8259536" cy="6111707"/>
+          <a:off x="9620250" y="40822"/>
+          <a:ext cx="12205608" cy="8079274"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1328,22 +1328,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
+      <xdr:colOff>312965</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>693965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>172657</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>775608</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>82418</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Slika 1">
+        <xdr:cNvPr id="6" name="Slika 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5048A12-C717-ABA1-9B3B-7A8F74BC3B5F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C5118B-2C12-6DCC-45AF-89AA3B3866A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,8 +1366,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9565822" y="149679"/>
-          <a:ext cx="12269406" cy="8096250"/>
+          <a:off x="9810751" y="8164286"/>
+          <a:ext cx="10395856" cy="5729382"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1666,19 +1666,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1691,39 +1691,39 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="56"/>
+      <c r="E5" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="57"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="46"/>
       <c r="G6" s="46"/>
       <c r="H6" s="46"/>
@@ -1734,7 +1734,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="45"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="46"/>
       <c r="G7" s="46"/>
       <c r="H7" s="46"/>
@@ -1745,7 +1745,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="57"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="46"/>
       <c r="G8" s="46"/>
       <c r="H8" s="46"/>
@@ -1756,7 +1756,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="57"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
@@ -1767,7 +1767,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="57"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="46"/>
       <c r="G10" s="46"/>
       <c r="H10" s="46"/>
@@ -1778,7 +1778,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="57"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
       <c r="H11" s="46"/>
@@ -1789,7 +1789,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="57"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="46"/>
       <c r="G12" s="46"/>
       <c r="H12" s="46"/>
@@ -1800,7 +1800,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="57"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
       <c r="H13" s="46"/>
@@ -1811,7 +1811,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="57"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="46"/>
       <c r="G14" s="46"/>
       <c r="H14" s="46"/>
@@ -1822,15 +1822,21 @@
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E8:J8"/>
@@ -1839,12 +1845,6 @@
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1855,8 +1855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB689FC-E53B-4F42-BD0A-17CBB93FB776}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,13 +1879,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="33">
         <v>0</v>
@@ -1912,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="37">
         <v>1</v>
@@ -1930,7 +1930,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="37">
         <v>2</v>
@@ -1945,7 +1945,7 @@
     <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="43"/>
       <c r="C6" s="44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18">
@@ -1964,7 +1964,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="41">
         <v>8</v>
@@ -2000,7 +2000,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="24">
         <v>16</v>
@@ -2018,7 +2018,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E10" s="24">
         <v>20</v>
@@ -2033,10 +2033,10 @@
     <row r="11" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="24">
         <v>24</v>
@@ -2054,7 +2054,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="24">
         <v>28</v>
@@ -2072,7 +2072,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="24">
         <v>29</v>
@@ -2087,10 +2087,10 @@
     <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="24">
         <v>30</v>
@@ -2105,10 +2105,10 @@
     <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>24</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>25</v>
       </c>
       <c r="E15" s="24">
         <v>94</v>
@@ -2123,10 +2123,10 @@
     <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="28" t="s">
         <v>30</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>31</v>
       </c>
       <c r="E16" s="29">
         <v>126</v>
@@ -2141,10 +2141,10 @@
     <row r="17" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="29">
         <v>134</v>
@@ -2159,7 +2159,7 @@
     <row r="18" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="21"/>
       <c r="C18" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="18">

</xml_diff>